<commit_message>
tambah fitur auto download saat export
</commit_message>
<xml_diff>
--- a/Data Export/Data Warga.xlsx
+++ b/Data Export/Data Warga.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
-  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xml:space="preserve">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView xWindow="90" yWindow="435" windowWidth="15015" windowHeight="4560"/>
+    <workbookView activeTab="0" autoFilterDateGrouping="true" firstSheet="0" minimized="false" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="600" visibility="visible"/>
   </bookViews>
   <sheets>
-    <sheet name="Worksheet" sheetId="1" r:id="rId1"/>
+    <sheet name="Worksheet" sheetId="1" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <definedNames/>
+  <calcPr calcId="999999" calcMode="auto" calcCompleted="1" fullCalcOnLoad="0" forceFullCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="121">
   <si>
     <t>No</t>
   </si>
@@ -199,6 +200,15 @@
     <t>6/10/1973</t>
   </si>
   <si>
+    <t>sdf</t>
+  </si>
+  <si>
+    <t>c</t>
+  </si>
+  <si>
+    <t>v</t>
+  </si>
+  <si>
     <t>PAULUS PATAR TUA PARDOSI</t>
   </si>
   <si>
@@ -211,6 +221,9 @@
     <t>4/1/1992</t>
   </si>
   <si>
+    <t>xcv</t>
+  </si>
+  <si>
     <t>JENTUMBUR SIHOMBING</t>
   </si>
   <si>
@@ -259,6 +272,9 @@
     <t>5/1/1994</t>
   </si>
   <si>
+    <t>xvc</t>
+  </si>
+  <si>
     <t>IDEO EDVANDITYA AGRITAMA</t>
   </si>
   <si>
@@ -307,6 +323,9 @@
     <t>5/23/1995</t>
   </si>
   <si>
+    <t>cxv</t>
+  </si>
+  <si>
     <t>WAYAN DAEM</t>
   </si>
   <si>
@@ -359,32 +378,19 @@
   </si>
   <si>
     <t>2/28/1985</t>
-  </si>
-  <si>
-    <t>sdf</t>
-  </si>
-  <si>
-    <t>v</t>
-  </si>
-  <si>
-    <t>c</t>
-  </si>
-  <si>
-    <t>xcv</t>
-  </si>
-  <si>
-    <t>xvc</t>
-  </si>
-  <si>
-    <t>cxv</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xml:space="preserve">
+  <numFmts count="0"/>
+  <fonts count="1">
     <font>
+      <b val="0"/>
+      <i val="0"/>
+      <strike val="0"/>
+      <u val="none"/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -395,17 +401,14 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="gray125"/>
+      <patternFill patternType="gray125">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
+    <border/>
     <border>
       <left style="thin">
         <color rgb="FF000000"/>
@@ -419,94 +422,24 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
-      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="1" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="0">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <tableStyles defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotTableStyle1"/>
 </styleSheet>
 </file>
 
@@ -515,10 +448,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="FFFFFF"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="1B1B1B"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -796,19 +729,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xml:space="preserve" mc:Ignorable="x14ac">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+  </sheetPr>
   <dimension ref="A1:AX26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AL16" workbookViewId="0">
-      <selection activeCell="AX23" sqref="AX23"/>
+    <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
+      <selection activeCell="A1" sqref="A1:AX26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="50" max="50" width="19.7109375" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
-    <row r="1" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:50">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -960,7 +893,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="2" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:50">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -1048,7 +981,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="3" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:50">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -1124,19 +1057,19 @@
       <c r="AS3" s="1"/>
       <c r="AT3" s="1"/>
       <c r="AU3" s="1" t="s">
-        <v>115</v>
+        <v>61</v>
       </c>
       <c r="AV3" s="1" t="s">
-        <v>115</v>
+        <v>61</v>
       </c>
       <c r="AW3" s="1" t="s">
-        <v>117</v>
+        <v>62</v>
       </c>
       <c r="AX3" s="1" t="s">
-        <v>116</v>
+        <v>63</v>
       </c>
     </row>
-    <row r="4" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:50">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -1155,7 +1088,7 @@
       </c>
       <c r="G4" s="1"/>
       <c r="H4" s="1" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="I4" s="1">
         <v>1</v>
@@ -1164,7 +1097,7 @@
         <v>52</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="L4" s="1">
         <v>4</v>
@@ -1216,7 +1149,7 @@
       <c r="AW4" s="1"/>
       <c r="AX4" s="1"/>
     </row>
-    <row r="5" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:50">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -1235,7 +1168,7 @@
       </c>
       <c r="G5" s="1"/>
       <c r="H5" s="1" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="I5" s="1">
         <v>1</v>
@@ -1244,7 +1177,7 @@
         <v>52</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="L5" s="1">
         <v>4</v>
@@ -1294,11 +1227,11 @@
       <c r="AU5" s="1"/>
       <c r="AV5" s="1"/>
       <c r="AW5" s="1" t="s">
-        <v>118</v>
+        <v>68</v>
       </c>
       <c r="AX5" s="1"/>
     </row>
-    <row r="6" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:50">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -1317,16 +1250,16 @@
       </c>
       <c r="G6" s="1"/>
       <c r="H6" s="1" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="I6" s="1">
         <v>1</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="L6" s="1">
         <v>1</v>
@@ -1378,7 +1311,7 @@
       <c r="AW6" s="1"/>
       <c r="AX6" s="1"/>
     </row>
-    <row r="7" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:50">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -1397,7 +1330,7 @@
       </c>
       <c r="G7" s="1"/>
       <c r="H7" s="1" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="I7" s="1">
         <v>1</v>
@@ -1406,7 +1339,7 @@
         <v>52</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="L7" s="1">
         <v>4</v>
@@ -1452,7 +1385,7 @@
       <c r="AQ7" s="1"/>
       <c r="AR7" s="1"/>
       <c r="AS7" s="1" t="s">
-        <v>118</v>
+        <v>68</v>
       </c>
       <c r="AT7" s="1"/>
       <c r="AU7" s="1"/>
@@ -1460,7 +1393,7 @@
       <c r="AW7" s="1"/>
       <c r="AX7" s="1"/>
     </row>
-    <row r="8" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:50">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -1479,16 +1412,16 @@
       </c>
       <c r="G8" s="1"/>
       <c r="H8" s="1" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="I8" s="1">
         <v>1</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="L8" s="1">
         <v>4</v>
@@ -1540,7 +1473,7 @@
       <c r="AW8" s="1"/>
       <c r="AX8" s="1"/>
     </row>
-    <row r="9" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:50">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -1559,16 +1492,16 @@
       </c>
       <c r="G9" s="1"/>
       <c r="H9" s="1" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="I9" s="1">
         <v>1</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="L9" s="1">
         <v>1</v>
@@ -1617,12 +1550,12 @@
       <c r="AT9" s="1"/>
       <c r="AU9" s="1"/>
       <c r="AV9" s="1" t="s">
-        <v>118</v>
+        <v>68</v>
       </c>
       <c r="AW9" s="1"/>
       <c r="AX9" s="1"/>
     </row>
-    <row r="10" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:50">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -1641,7 +1574,7 @@
       </c>
       <c r="G10" s="1"/>
       <c r="H10" s="1" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="I10" s="1">
         <v>1</v>
@@ -1650,7 +1583,7 @@
         <v>59</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="L10" s="1">
         <v>1</v>
@@ -1702,7 +1635,7 @@
       <c r="AW10" s="1"/>
       <c r="AX10" s="1"/>
     </row>
-    <row r="11" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:50">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -1721,16 +1654,16 @@
       </c>
       <c r="G11" s="1"/>
       <c r="H11" s="1" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="I11" s="1">
         <v>1</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="K11" s="1" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="L11" s="1">
         <v>4</v>
@@ -1778,15 +1711,15 @@
       <c r="AS11" s="1"/>
       <c r="AT11" s="1"/>
       <c r="AU11" s="1" t="s">
-        <v>118</v>
+        <v>68</v>
       </c>
       <c r="AV11" s="1"/>
       <c r="AW11" s="1" t="s">
-        <v>119</v>
+        <v>85</v>
       </c>
       <c r="AX11" s="1"/>
     </row>
-    <row r="12" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:50">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -1805,16 +1738,16 @@
       </c>
       <c r="G12" s="1"/>
       <c r="H12" s="1" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="I12" s="1">
         <v>1</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="K12" s="1" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="L12" s="1">
         <v>4</v>
@@ -1863,12 +1796,12 @@
       <c r="AT12" s="1"/>
       <c r="AU12" s="1"/>
       <c r="AV12" s="1" t="s">
-        <v>118</v>
+        <v>68</v>
       </c>
       <c r="AW12" s="1"/>
       <c r="AX12" s="1"/>
     </row>
-    <row r="13" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:50">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -1887,16 +1820,16 @@
       </c>
       <c r="G13" s="1"/>
       <c r="H13" s="1" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="I13" s="1">
         <v>1</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="K13" s="1" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="L13" s="1">
         <v>4</v>
@@ -1948,7 +1881,7 @@
       <c r="AW13" s="1"/>
       <c r="AX13" s="1"/>
     </row>
-    <row r="14" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:50">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -1967,7 +1900,7 @@
       </c>
       <c r="G14" s="1"/>
       <c r="H14" s="1" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="I14" s="1">
         <v>1</v>
@@ -1976,7 +1909,7 @@
         <v>59</v>
       </c>
       <c r="K14" s="1" t="s">
-        <v>88</v>
+        <v>93</v>
       </c>
       <c r="L14" s="1">
         <v>1</v>
@@ -2027,10 +1960,10 @@
       <c r="AV14" s="1"/>
       <c r="AW14" s="1"/>
       <c r="AX14" s="1" t="s">
-        <v>118</v>
+        <v>68</v>
       </c>
     </row>
-    <row r="15" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:50">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -2049,7 +1982,7 @@
       </c>
       <c r="G15" s="1"/>
       <c r="H15" s="1" t="s">
-        <v>89</v>
+        <v>94</v>
       </c>
       <c r="I15" s="1">
         <v>1</v>
@@ -2058,7 +1991,7 @@
         <v>52</v>
       </c>
       <c r="K15" s="1" t="s">
-        <v>90</v>
+        <v>95</v>
       </c>
       <c r="L15" s="1">
         <v>4</v>
@@ -2110,7 +2043,7 @@
       <c r="AW15" s="1"/>
       <c r="AX15" s="1"/>
     </row>
-    <row r="16" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:50">
       <c r="A16" s="1">
         <v>15</v>
       </c>
@@ -2129,7 +2062,7 @@
       </c>
       <c r="G16" s="1"/>
       <c r="H16" s="1" t="s">
-        <v>91</v>
+        <v>96</v>
       </c>
       <c r="I16" s="1">
         <v>1</v>
@@ -2138,7 +2071,7 @@
         <v>59</v>
       </c>
       <c r="K16" s="1" t="s">
-        <v>92</v>
+        <v>97</v>
       </c>
       <c r="L16" s="1">
         <v>1</v>
@@ -2190,7 +2123,7 @@
       <c r="AW16" s="1"/>
       <c r="AX16" s="1"/>
     </row>
-    <row r="17" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:50">
       <c r="A17" s="1">
         <v>16</v>
       </c>
@@ -2209,16 +2142,16 @@
       </c>
       <c r="G17" s="1"/>
       <c r="H17" s="1" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="I17" s="1">
         <v>1</v>
       </c>
       <c r="J17" s="1" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="K17" s="1" t="s">
-        <v>94</v>
+        <v>99</v>
       </c>
       <c r="L17" s="1">
         <v>1</v>
@@ -2270,7 +2203,7 @@
       <c r="AW17" s="1"/>
       <c r="AX17" s="1"/>
     </row>
-    <row r="18" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:50">
       <c r="A18" s="1">
         <v>17</v>
       </c>
@@ -2289,7 +2222,7 @@
       </c>
       <c r="G18" s="1"/>
       <c r="H18" s="1" t="s">
-        <v>95</v>
+        <v>100</v>
       </c>
       <c r="I18" s="1">
         <v>1</v>
@@ -2298,7 +2231,7 @@
         <v>59</v>
       </c>
       <c r="K18" s="1" t="s">
-        <v>96</v>
+        <v>101</v>
       </c>
       <c r="L18" s="1">
         <v>4</v>
@@ -2345,18 +2278,18 @@
       <c r="AR18" s="1"/>
       <c r="AS18" s="1"/>
       <c r="AT18" s="1" t="s">
-        <v>119</v>
+        <v>85</v>
       </c>
       <c r="AU18" s="1"/>
       <c r="AV18" s="1" t="s">
-        <v>120</v>
+        <v>102</v>
       </c>
       <c r="AW18" s="1" t="s">
-        <v>118</v>
+        <v>68</v>
       </c>
       <c r="AX18" s="1"/>
     </row>
-    <row r="19" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:50">
       <c r="A19" s="1">
         <v>18</v>
       </c>
@@ -2375,16 +2308,16 @@
       </c>
       <c r="G19" s="1"/>
       <c r="H19" s="1" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="I19" s="1">
         <v>1</v>
       </c>
       <c r="J19" s="1" t="s">
-        <v>98</v>
+        <v>104</v>
       </c>
       <c r="K19" s="1" t="s">
-        <v>99</v>
+        <v>105</v>
       </c>
       <c r="L19" s="1">
         <v>1</v>
@@ -2436,7 +2369,7 @@
       <c r="AW19" s="1"/>
       <c r="AX19" s="1"/>
     </row>
-    <row r="20" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:50">
       <c r="A20" s="1">
         <v>19</v>
       </c>
@@ -2455,7 +2388,7 @@
       </c>
       <c r="G20" s="1"/>
       <c r="H20" s="1" t="s">
-        <v>100</v>
+        <v>106</v>
       </c>
       <c r="I20" s="1">
         <v>1</v>
@@ -2464,7 +2397,7 @@
         <v>59</v>
       </c>
       <c r="K20" s="1" t="s">
-        <v>101</v>
+        <v>107</v>
       </c>
       <c r="L20" s="1">
         <v>1</v>
@@ -2509,7 +2442,7 @@
       <c r="AP20" s="1"/>
       <c r="AQ20" s="1"/>
       <c r="AR20" s="1" t="s">
-        <v>118</v>
+        <v>68</v>
       </c>
       <c r="AS20" s="1"/>
       <c r="AT20" s="1"/>
@@ -2518,7 +2451,7 @@
       <c r="AW20" s="1"/>
       <c r="AX20" s="1"/>
     </row>
-    <row r="21" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:50">
       <c r="A21" s="1">
         <v>20</v>
       </c>
@@ -2537,7 +2470,7 @@
       </c>
       <c r="G21" s="1"/>
       <c r="H21" s="1" t="s">
-        <v>102</v>
+        <v>108</v>
       </c>
       <c r="I21" s="1">
         <v>1</v>
@@ -2546,7 +2479,7 @@
         <v>52</v>
       </c>
       <c r="K21" s="1" t="s">
-        <v>103</v>
+        <v>109</v>
       </c>
       <c r="L21" s="1">
         <v>4</v>
@@ -2598,7 +2531,7 @@
       <c r="AW21" s="1"/>
       <c r="AX21" s="1"/>
     </row>
-    <row r="22" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:50">
       <c r="A22" s="1">
         <v>21</v>
       </c>
@@ -2617,7 +2550,7 @@
       </c>
       <c r="G22" s="1"/>
       <c r="H22" s="1" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="I22" s="1">
         <v>1</v>
@@ -2626,7 +2559,7 @@
         <v>59</v>
       </c>
       <c r="K22" s="1" t="s">
-        <v>105</v>
+        <v>111</v>
       </c>
       <c r="L22" s="1">
         <v>4</v>
@@ -2678,7 +2611,7 @@
       <c r="AW22" s="1"/>
       <c r="AX22" s="1"/>
     </row>
-    <row r="23" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:50">
       <c r="A23" s="1">
         <v>22</v>
       </c>
@@ -2697,16 +2630,16 @@
       </c>
       <c r="G23" s="1"/>
       <c r="H23" s="1" t="s">
-        <v>106</v>
+        <v>112</v>
       </c>
       <c r="I23" s="1">
         <v>1</v>
       </c>
       <c r="J23" s="1" t="s">
-        <v>98</v>
+        <v>104</v>
       </c>
       <c r="K23" s="1" t="s">
-        <v>107</v>
+        <v>113</v>
       </c>
       <c r="L23" s="1">
         <v>1</v>
@@ -2751,7 +2684,7 @@
       <c r="AP23" s="1"/>
       <c r="AQ23" s="1"/>
       <c r="AR23" s="1" t="s">
-        <v>118</v>
+        <v>68</v>
       </c>
       <c r="AS23" s="1"/>
       <c r="AT23" s="1"/>
@@ -2760,7 +2693,7 @@
       <c r="AW23" s="1"/>
       <c r="AX23" s="1"/>
     </row>
-    <row r="24" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:50">
       <c r="A24" s="1">
         <v>23</v>
       </c>
@@ -2779,16 +2712,16 @@
       </c>
       <c r="G24" s="1"/>
       <c r="H24" s="1" t="s">
-        <v>108</v>
+        <v>114</v>
       </c>
       <c r="I24" s="1">
         <v>1</v>
       </c>
       <c r="J24" s="1" t="s">
-        <v>98</v>
+        <v>104</v>
       </c>
       <c r="K24" s="1" t="s">
-        <v>109</v>
+        <v>115</v>
       </c>
       <c r="L24" s="1">
         <v>1</v>
@@ -2835,16 +2768,16 @@
       <c r="AR24" s="1"/>
       <c r="AS24" s="1"/>
       <c r="AT24" s="1" t="s">
-        <v>119</v>
+        <v>85</v>
       </c>
       <c r="AU24" s="1"/>
       <c r="AV24" s="1"/>
       <c r="AW24" s="1"/>
       <c r="AX24" s="1" t="s">
-        <v>116</v>
+        <v>63</v>
       </c>
     </row>
-    <row r="25" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:50">
       <c r="A25" s="1">
         <v>24</v>
       </c>
@@ -2863,16 +2796,16 @@
       </c>
       <c r="G25" s="1"/>
       <c r="H25" s="1" t="s">
-        <v>110</v>
+        <v>116</v>
       </c>
       <c r="I25" s="1">
         <v>1</v>
       </c>
       <c r="J25" s="1" t="s">
-        <v>111</v>
+        <v>117</v>
       </c>
       <c r="K25" s="1" t="s">
-        <v>112</v>
+        <v>118</v>
       </c>
       <c r="L25" s="1">
         <v>1</v>
@@ -2921,12 +2854,12 @@
       <c r="AT25" s="1"/>
       <c r="AU25" s="1"/>
       <c r="AV25" s="1" t="s">
-        <v>119</v>
+        <v>85</v>
       </c>
       <c r="AW25" s="1"/>
       <c r="AX25" s="1"/>
     </row>
-    <row r="26" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:50">
       <c r="A26" s="1">
         <v>25</v>
       </c>
@@ -2945,7 +2878,7 @@
       </c>
       <c r="G26" s="1"/>
       <c r="H26" s="1" t="s">
-        <v>113</v>
+        <v>119</v>
       </c>
       <c r="I26" s="1">
         <v>1</v>
@@ -2954,7 +2887,7 @@
         <v>59</v>
       </c>
       <c r="K26" s="1" t="s">
-        <v>114</v>
+        <v>120</v>
       </c>
       <c r="L26" s="1">
         <v>4</v>
@@ -3023,7 +2956,17 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
+  <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>
+  <printOptions gridLines="false" gridLinesSet="true"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="1" orientation="default" scale="100" fitToHeight="1" fitToWidth="1"/>
+  <headerFooter differentOddEven="false" differentFirst="false" scaleWithDoc="true" alignWithMargins="true">
+    <oddHeader/>
+    <oddFooter/>
+    <evenHeader/>
+    <evenFooter/>
+    <firstHeader/>
+    <firstFooter/>
+  </headerFooter>
 </worksheet>
 </file>
</xml_diff>